<commit_message>
update dependent select2, fix raf sum
</commit_message>
<xml_diff>
--- a/public/Master Order Master.xlsx
+++ b/public/Master Order Master.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="40">
   <si>
     <t>No</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Sketch File</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
   <si>
     <t>ORM000000001</t>
@@ -1079,10 +1082,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:O7"/>
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6"/>
@@ -1101,7 +1104,7 @@
     <col min="15" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1146,6 +1149,9 @@
       </c>
       <c r="O1" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -1153,22 +1159,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H2" s="1">
         <v>149184</v>
@@ -1183,16 +1189,16 @@
         <v>149296</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -1200,22 +1206,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H3" s="1">
         <v>20448</v>
@@ -1230,16 +1236,16 @@
         <v>20138</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -1247,22 +1253,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H4" s="1">
         <v>67212</v>
@@ -1271,22 +1277,22 @@
         <v>67212</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K4" s="1">
         <v>67290</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -1294,22 +1300,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H5" s="1">
         <v>117240</v>
@@ -1324,16 +1330,16 @@
         <v>111334</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -1341,22 +1347,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H6" s="1">
         <v>11700</v>
@@ -1371,16 +1377,16 @@
         <v>11678</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -1388,22 +1394,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H7" s="1">
         <v>65772</v>
@@ -1418,16 +1424,16 @@
         <v>65734</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>